<commit_message>
update BOM £10.36 each
</commit_message>
<xml_diff>
--- a/RcCtlHwParts.xlsx
+++ b/RcCtlHwParts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RC\RC8266Controller\RcCtlHw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RC\RC8266Controller\PCB_RcCtl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0D3A47-19A0-41DE-88A4-D1808F84D02C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD7BE85-0B81-440D-BD8E-00A04F0FF783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="1560" windowWidth="24060" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="2490" windowWidth="21645" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>J1</t>
   </si>
@@ -99,9 +99,6 @@
     <t>V1</t>
   </si>
   <si>
-    <t>BA033</t>
-  </si>
-  <si>
     <t>3V3 regulator</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>MIC5365-2.8YCR-TR</t>
-  </si>
-  <si>
     <t>SC-70-5</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>R1,3</t>
   </si>
   <si>
-    <t>R4,5,6,7,8</t>
-  </si>
-  <si>
     <t>10K Resistor</t>
   </si>
   <si>
@@ -208,13 +199,49 @@
   </si>
   <si>
     <t>5mm</t>
+  </si>
+  <si>
+    <t>R6,7,8</t>
+  </si>
+  <si>
+    <t>BA033CC0FP-E2</t>
+  </si>
+  <si>
+    <t>MIC5365-2.8YC5-TR</t>
+  </si>
+  <si>
+    <t>MCWR08X1201FTL</t>
+  </si>
+  <si>
+    <t>WW25PR400FTL</t>
+  </si>
+  <si>
+    <t>C2012X6S1A106K085AC</t>
+  </si>
+  <si>
+    <t>652338 6.5*23*38mm</t>
+  </si>
+  <si>
+    <t>TXT LCD</t>
+  </si>
+  <si>
+    <t>2074334</t>
+  </si>
+  <si>
+    <t>MC0805B104M500CT</t>
+  </si>
+  <si>
+    <t>BangGood</t>
+  </si>
+  <si>
+    <t>Ebay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +252,14 @@
     <font>
       <b/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -252,10 +287,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,24 +573,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -573,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
@@ -604,6 +641,9 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
       <c r="G2" t="s">
         <v>7</v>
       </c>
@@ -611,11 +651,11 @@
         <v>20</v>
       </c>
       <c r="I2">
-        <v>2.15</v>
+        <v>0.76</v>
       </c>
       <c r="J2">
         <f>I2/H2*E2</f>
-        <v>0.1075</v>
+        <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -635,7 +675,20 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J3">
+        <f>I3/H3*E3</f>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -654,6 +707,9 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
       <c r="G4" t="s">
         <v>7</v>
       </c>
@@ -661,11 +717,12 @@
         <v>5</v>
       </c>
       <c r="I4">
-        <v>7.68</v>
+        <f xml:space="preserve"> 0.87 * 5</f>
+        <v>4.3499999999999996</v>
       </c>
       <c r="J4">
         <f>I4/H4*E4</f>
-        <v>1.536</v>
+        <v>0.86999999999999988</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -673,56 +730,82 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0.87</v>
+      </c>
+      <c r="J5">
+        <f>I5/H5*E5</f>
+        <v>0.87</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
       <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J6">
+        <f>I6/H6*E6</f>
+        <v>0.11200000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
@@ -740,132 +823,257 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J8">
+        <f>I8/H8*E8</f>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>3.75</v>
+      </c>
+      <c r="J9">
+        <f>I9/H9*E9</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10">
+        <f>10</f>
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f>10*0.0195</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="J10">
+        <f>I10/H10*E10</f>
+        <v>9.7500000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>0.54</v>
+      </c>
+      <c r="J11">
+        <f>I11/H11*E11</f>
+        <v>0.21600000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <f>10*0.052</f>
+        <v>0.52</v>
+      </c>
+      <c r="J12">
+        <f>I12/H12*E12</f>
+        <v>0.10400000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="J13">
+        <f>I13/H13*E13</f>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
         <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>2.44</v>
+      </c>
+      <c r="J14">
+        <f>I14/H14*E14</f>
+        <v>0.24399999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="J15">
+        <f>I15/H15*E15</f>
+        <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -875,42 +1083,119 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
       <c r="F16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>1.31</v>
+      </c>
+      <c r="J16">
+        <f>I16/H16*E16</f>
+        <v>0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="3">
+        <f>1/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>1.63</v>
+      </c>
+      <c r="J17">
+        <f>I17/H17*E17</f>
+        <v>2.0374999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>54</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
       <c r="E18">
         <v>1</v>
       </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>0.86</v>
+      </c>
+      <c r="J18">
+        <f>I18/H18*E18</f>
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <f>1.33*2</f>
+        <v>2.66</v>
+      </c>
+      <c r="J19">
+        <f>I19/H19*E19</f>
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="4">
+        <f>SUM(J2:J19)</f>
+        <v>10.357775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update BOM spreadsheet with current stock
</commit_message>
<xml_diff>
--- a/RcCtlHwParts.xlsx
+++ b/RcCtlHwParts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RC\RC8266Controller\PCB_RcCtl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD7BE85-0B81-440D-BD8E-00A04F0FF783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C8EFC0-450B-454B-823B-08AE7A0B6FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="2490" windowWidth="21645" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1965" yWindow="2430" windowWidth="21645" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>J1</t>
   </si>
@@ -222,9 +222,6 @@
     <t>652338 6.5*23*38mm</t>
   </si>
   <si>
-    <t>TXT LCD</t>
-  </si>
-  <si>
     <t>2074334</t>
   </si>
   <si>
@@ -235,6 +232,27 @@
   </si>
   <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>got</t>
+  </si>
+  <si>
+    <t>onorder</t>
+  </si>
+  <si>
+    <t>lots</t>
+  </si>
+  <si>
+    <t>0.96" 80x160 IPS TFT</t>
+  </si>
+  <si>
+    <t>sipeed langan nano</t>
+  </si>
+  <si>
+    <t>aliexpress</t>
+  </si>
+  <si>
+    <t>farnell</t>
   </si>
 </sst>
 </file>
@@ -573,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +611,7 @@
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -624,8 +642,14 @@
       <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -654,11 +678,14 @@
         <v>0.76</v>
       </c>
       <c r="J2">
-        <f>I2/H2*E2</f>
+        <f t="shared" ref="J2:J19" si="0">I2/H2*E2</f>
         <v>3.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -687,11 +714,14 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="J3">
-        <f>I3/H3*E3</f>
+        <f t="shared" si="0"/>
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -721,11 +751,20 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="J4">
-        <f>I4/H4*E4</f>
+        <f t="shared" si="0"/>
         <v>0.86999999999999988</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -754,11 +793,20 @@
         <v>0.87</v>
       </c>
       <c r="J5">
-        <f>I5/H5*E5</f>
+        <f t="shared" si="0"/>
         <v>0.87</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -787,11 +835,20 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="J6">
-        <f>I6/H6*E6</f>
+        <f t="shared" si="0"/>
         <v>0.11200000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -817,11 +874,14 @@
         <v>7.19</v>
       </c>
       <c r="J7">
-        <f>I7/H7*E7</f>
+        <f t="shared" si="0"/>
         <v>7.1900000000000006E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -850,11 +910,14 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="J8">
-        <f>I8/H8*E8</f>
+        <f t="shared" si="0"/>
         <v>1.6E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -883,11 +946,14 @@
         <v>3.75</v>
       </c>
       <c r="J9">
-        <f>I9/H9*E9</f>
+        <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -895,7 +961,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>37</v>
@@ -918,11 +984,14 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="J10">
-        <f>I10/H10*E10</f>
+        <f t="shared" si="0"/>
         <v>9.7500000000000003E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -951,11 +1020,20 @@
         <v>0.54</v>
       </c>
       <c r="J11">
-        <f>I11/H11*E11</f>
+        <f t="shared" si="0"/>
         <v>0.21600000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -963,7 +1041,7 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>37</v>
@@ -985,11 +1063,14 @@
         <v>0.52</v>
       </c>
       <c r="J12">
-        <f>I12/H12*E12</f>
+        <f t="shared" si="0"/>
         <v>0.10400000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1016,11 +1097,14 @@
         <v>4.6399999999999997</v>
       </c>
       <c r="J13">
-        <f>I13/H13*E13</f>
+        <f t="shared" si="0"/>
         <v>2.3199999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1035,7 +1119,7 @@
         <v>29</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -1044,11 +1128,14 @@
         <v>2.44</v>
       </c>
       <c r="J14">
-        <f>I14/H14*E14</f>
+        <f t="shared" si="0"/>
         <v>0.24399999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1063,7 +1150,7 @@
         <v>29</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1072,11 +1159,20 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="J15">
-        <f>I15/H15*E15</f>
+        <f t="shared" si="0"/>
         <v>2.2599999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +1186,7 @@
         <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H16">
         <v>10</v>
@@ -1099,11 +1195,14 @@
         <v>1.31</v>
       </c>
       <c r="J16">
-        <f>I16/H16*E16</f>
+        <f t="shared" si="0"/>
         <v>0.13100000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1121,7 +1220,7 @@
         <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H17">
         <v>10</v>
@@ -1130,11 +1229,14 @@
         <v>1.63</v>
       </c>
       <c r="J17">
-        <f>I17/H17*E17</f>
+        <f t="shared" si="0"/>
         <v>2.0374999999999997E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1160,16 +1262,25 @@
         <v>0.86</v>
       </c>
       <c r="J18">
-        <f>I18/H18*E18</f>
+        <f t="shared" si="0"/>
         <v>0.17199999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+      <c r="N18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1188,11 +1299,20 @@
         <v>2.66</v>
       </c>
       <c r="J19">
-        <f>I19/H19*E19</f>
+        <f t="shared" si="0"/>
         <v>1.33</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J20" s="4">
         <f>SUM(J2:J19)</f>
         <v>10.357775</v>

</xml_diff>